<commit_message>
Added F1 in py.
</commit_message>
<xml_diff>
--- a/docs/anomaly_detection/result_new.xlsx
+++ b/docs/anomaly_detection/result_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95346063eca47658/documents/computerScience/RIT/2023 spring/NetworkingResearch/inswitch_anomaly/docs/anomaly_detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="811" documentId="13_ncr:1_{1CBB4632-0BF8-440C-8894-48E6D8A48BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90E71D97-E655-4A6D-985F-07BE3D765BC0}"/>
+  <xr:revisionPtr revIDLastSave="812" documentId="13_ncr:1_{1CBB4632-0BF8-440C-8894-48E6D8A48BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{721DF652-2CD9-4CC8-9CA6-AEF511CCC88C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2832" yWindow="3444" windowWidth="17280" windowHeight="10500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No P4 &amp; lim4 &amp; no-bala" sheetId="13" r:id="rId1"/>
@@ -768,7 +768,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,7 +832,9 @@
       <c r="D4" s="1">
         <v>94.238919768704704</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>97.201099999999997</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added confusion_matrix in py
</commit_message>
<xml_diff>
--- a/docs/anomaly_detection/result_new.xlsx
+++ b/docs/anomaly_detection/result_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95346063eca47658/documents/computerScience/RIT/2023 spring/NetworkingResearch/inswitch_anomaly/docs/anomaly_detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="812" documentId="13_ncr:1_{1CBB4632-0BF8-440C-8894-48E6D8A48BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{721DF652-2CD9-4CC8-9CA6-AEF511CCC88C}"/>
+  <xr:revisionPtr revIDLastSave="969" documentId="13_ncr:1_{1CBB4632-0BF8-440C-8894-48E6D8A48BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C32CCD9-0DBA-424A-B857-5125CE3E7BA1}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="3444" windowWidth="17280" windowHeight="10500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No P4 &amp; lim4 &amp; no-bala" sheetId="13" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>BoT-IoT</t>
   </si>
@@ -54,13 +54,28 @@
     <t>Use balaned original data sets to train and but origianl data sets to test, no synthesized good pkts added.</t>
   </si>
   <si>
-    <t>1(py)</t>
-  </si>
-  <si>
-    <t>1(p4)</t>
-  </si>
-  <si>
     <t>(Both py and p4)Sketch limitation of 8, meaning 8 spots for src ip and dst ip, separately.</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1Score</t>
+  </si>
+  <si>
+    <t>BoT-IoT 1</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>py</t>
   </si>
 </sst>
 </file>
@@ -76,7 +91,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,8 +110,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -237,11 +258,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -278,12 +326,53 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -765,10 +854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DC7AE6-5869-4AAF-8061-4BCD894E7315}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,116 +865,284 @@
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="29"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="2">
+      <c r="B3" s="28">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="19">
+        <v>0.97909999999999997</v>
+      </c>
+      <c r="E3" s="19">
+        <v>94.24</v>
+      </c>
+      <c r="H3" s="26"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.1414</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0.64980000000000004</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="H6" s="26"/>
+      <c r="J6" s="24"/>
+      <c r="L6" s="24"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28">
+        <v>3</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.99619999999999997</v>
+      </c>
+      <c r="E7" s="19">
+        <v>97.201099999999997</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="J7" s="24"/>
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="19">
+        <v>1.83E-2</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0.66359999999999997</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="19">
+        <v>3.56E-2</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="H10" s="25"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28">
+        <v>4</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.98680000000000001</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0.96819299999999997</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="19">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="E12" s="19">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="H12" s="20"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="19">
+        <v>0.68369999999999997</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0.96809999999999996</v>
+      </c>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0.98380000000000001</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C15" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1">
-        <v>99.51</v>
-      </c>
-      <c r="E3" s="1">
-        <v>99.61</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="2" t="s">
+      <c r="D15" s="19">
+        <v>0.99770000000000003</v>
+      </c>
+      <c r="E15" s="19">
+        <v>0.97230000000000005</v>
+      </c>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="19">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="E16" s="19">
+        <v>1</v>
+      </c>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0.72</v>
+      </c>
+      <c r="E17" s="19">
+        <v>0.97230000000000005</v>
+      </c>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4.48E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.9859</v>
+      </c>
+      <c r="H18" s="25"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1">
-        <v>94.238919768704704</v>
-      </c>
-      <c r="E4" s="1">
-        <v>97.201099999999997</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A3:A7"/>
+  <mergeCells count="6">
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B7:B10"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:G7">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>80</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>